<commit_message>
Fix for test issues that occured running Tox.
</commit_message>
<xml_diff>
--- a/tests/fixtures/functions.xlsx
+++ b/tests/fixtures/functions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tarkm\PycharmProjects\PyxlOptimizer\tests\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28785EE9-05A9-4F6A-9624-5E3683A3FBF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{599ADFEC-A19D-4316-8E81-B35F8B3DF1A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" tabRatio="744" activeTab="7" xr2:uid="{339F090E-C415-4B76-9E24-B80EB581BF8C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" tabRatio="744" xr2:uid="{339F090E-C415-4B76-9E24-B80EB581BF8C}"/>
   </bookViews>
   <sheets>
     <sheet name="Average" sheetId="10" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -1026,16 +1026,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD2A8D8C-4735-4892-B1D7-7BD45555EA76}">
   <dimension ref="A1:T11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="V16" sqref="V16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.86328125" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1047,7 +1047,7 @@
       </c>
       <c r="P1" s="3"/>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>41</v>
       </c>
@@ -1076,7 +1076,7 @@
       </c>
       <c r="P2" s="3"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>42</v>
       </c>
@@ -1120,32 +1120,28 @@
       </c>
       <c r="P3" s="3"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
       <c r="C4">
-        <f>AVERAGEIFS(D4:H4,J4:N4,TRUE,P4:T4,TRUE)</f>
-        <v>3.5</v>
-      </c>
-      <c r="D4">
-        <v>4</v>
+        <v>2</v>
+      </c>
+      <c r="D4" t="e">
+        <f>AVERAGEIFS(E4:H4,J4:N4,TRUE,P4:T4,TRUE)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4">
         <v>5</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>6</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>7</v>
-      </c>
-      <c r="H4">
-        <f>B4</f>
-        <v>2</v>
       </c>
       <c r="J4" t="b">
         <v>0</v>
@@ -1178,7 +1174,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>43</v>
       </c>
@@ -1206,7 +1202,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>44</v>
       </c>
@@ -1237,7 +1233,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>45</v>
       </c>
@@ -1268,7 +1264,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>46</v>
       </c>
@@ -1296,7 +1292,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>47</v>
       </c>
@@ -1324,7 +1320,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>48</v>
       </c>
@@ -1352,7 +1348,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="H11">
         <f>B11</f>
         <v>0</v>
@@ -1370,12 +1366,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.3984375" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1386,7 +1382,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>35</v>
       </c>
@@ -1414,7 +1410,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>36</v>
       </c>
@@ -1442,7 +1438,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>37</v>
       </c>
@@ -1470,7 +1466,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>38</v>
       </c>
@@ -1482,7 +1478,7 @@
         <v>1.4142135623730951</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>39</v>
       </c>
@@ -1494,7 +1490,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>40</v>
       </c>
@@ -1506,17 +1502,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>162</v>
       </c>
@@ -1544,7 +1540,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>163</v>
       </c>
@@ -1572,7 +1568,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>164</v>
       </c>
@@ -1600,7 +1596,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>165</v>
       </c>
@@ -1628,7 +1624,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>166</v>
       </c>
@@ -1640,7 +1636,7 @@
         <v>260.88676080802708</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>147</v>
       </c>
@@ -1652,7 +1648,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>148</v>
       </c>
@@ -1664,7 +1660,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>149</v>
       </c>
@@ -1679,7 +1675,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>150</v>
       </c>
@@ -1694,7 +1690,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>151</v>
       </c>
@@ -1706,7 +1702,7 @@
         <v>1022415</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>152</v>
       </c>
@@ -1718,7 +1714,7 @@
         <v>3267</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>153</v>
       </c>
@@ -1730,7 +1726,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>154</v>
       </c>
@@ -1742,17 +1738,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>157</v>
       </c>
@@ -1764,7 +1760,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>158</v>
       </c>
@@ -1776,7 +1772,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>159</v>
       </c>
@@ -1808,12 +1804,12 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.265625" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1824,7 +1820,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>167</v>
       </c>
@@ -1836,7 +1832,7 @@
         <v>-245.20000000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>168</v>
       </c>
@@ -1848,7 +1844,7 @@
         <v>-245.20000000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>169</v>
       </c>
@@ -1860,7 +1856,7 @@
         <v>-245.20000000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>170</v>
       </c>
@@ -1872,7 +1868,7 @@
         <v>-245.20000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>171</v>
       </c>
@@ -1884,7 +1880,7 @@
         <v>-246</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>172</v>
       </c>
@@ -1896,7 +1892,7 @@
         <v>-245.3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>173</v>
       </c>
@@ -1908,7 +1904,7 @@
         <v>-245.3</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>174</v>
       </c>
@@ -1920,7 +1916,7 @@
         <v>-245.3</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>175</v>
       </c>
@@ -1932,7 +1928,7 @@
         <v>-246</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>176</v>
       </c>
@@ -1944,7 +1940,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>177</v>
       </c>
@@ -1956,7 +1952,7 @@
         <v>-247</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>178</v>
       </c>
@@ -1968,7 +1964,7 @@
         <v>-245.2</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>179</v>
       </c>
@@ -1980,7 +1976,7 @@
         <v>-245.2</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>180</v>
       </c>
@@ -1992,7 +1988,7 @@
         <v>-245.29999999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>181</v>
       </c>
@@ -2017,14 +2013,14 @@
       <selection activeCell="B28" sqref="B28:K28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.3984375" customWidth="1"/>
-    <col min="2" max="2" width="22.86328125" customWidth="1"/>
-    <col min="3" max="3" width="15.1328125" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2035,7 +2031,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>51</v>
       </c>
@@ -2050,7 +2046,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>53</v>
       </c>
@@ -2062,7 +2058,7 @@
         <v>Hello Goodye</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>52</v>
       </c>
@@ -2074,7 +2070,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>54</v>
       </c>
@@ -2086,7 +2082,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>55</v>
       </c>
@@ -2098,7 +2094,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>60</v>
       </c>
@@ -2110,7 +2106,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>56</v>
       </c>
@@ -2122,7 +2118,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>61</v>
       </c>
@@ -2134,7 +2130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>67</v>
       </c>
@@ -2146,7 +2142,7 @@
         <v>test string</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>68</v>
       </c>
@@ -2158,7 +2154,7 @@
         <v>Test String</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>69</v>
       </c>
@@ -2170,7 +2166,7 @@
         <v>TEST STRING</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>70</v>
       </c>
@@ -2182,7 +2178,7 @@
         <v>42.24</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>71</v>
       </c>
@@ -2194,7 +2190,7 @@
         <v>A</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>72</v>
       </c>
@@ -2206,7 +2202,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>73</v>
       </c>
@@ -2218,7 +2214,7 @@
         <v>帻</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>84</v>
       </c>
@@ -2230,7 +2226,7 @@
         <v>24123</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>74</v>
       </c>
@@ -2245,7 +2241,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>75</v>
       </c>
@@ -2260,7 +2256,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>76</v>
       </c>
@@ -2272,7 +2268,7 @@
         <v>Test</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>77</v>
       </c>
@@ -2284,7 +2280,7 @@
         <v>est s</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>78</v>
       </c>
@@ -2296,7 +2292,7 @@
         <v>string</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>185</v>
       </c>
@@ -2324,7 +2320,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>186</v>
       </c>
@@ -2352,7 +2348,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>79</v>
       </c>
@@ -2364,7 +2360,7 @@
         <v>TLong new random stringtring</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>80</v>
       </c>
@@ -2390,9 +2386,9 @@
       <selection sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2403,7 +2399,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2415,7 +2411,7 @@
         <v>6.2831853071795862</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -2427,7 +2423,7 @@
         <v>2.5066282746310002</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -2439,7 +2435,7 @@
         <v>114.59155902616465</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -2451,7 +2447,7 @@
         <v>3.4906585039886591E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -2463,7 +2459,7 @@
         <v>-0.41614683654714241</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -2475,7 +2471,7 @@
         <v>1.4644929324746168</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -2487,7 +2483,7 @@
         <v>3.7621956910836314</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -2499,7 +2495,7 @@
         <v>1.3169578969248166</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -2511,7 +2507,7 @@
         <v>-2.4029979617223809</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -2523,7 +2519,7 @@
         <v>0.26580222883407972</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -2535,7 +2531,7 @@
         <v>0.90929742682568171</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -2547,7 +2543,7 @@
         <v>0.10630339432027981</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -2559,7 +2555,7 @@
         <v>1.4436354751788103</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -2571,7 +2567,7 @@
         <v>1.0997501702946164</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -2583,7 +2579,7 @@
         <v>0.27572056477178319</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -2595,7 +2591,7 @@
         <v>-2.1850398632615189</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -2607,7 +2603,7 @@
         <v>1.1071487177940904</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -2619,7 +2615,7 @@
         <v>0.78539816339744828</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -2631,7 +2627,7 @@
         <v>1.3526254688173596</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -2643,7 +2639,7 @@
         <v>1.0373147207275479</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -2655,7 +2651,7 @@
         <v>1.0038848218538872</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -2681,9 +2677,9 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2694,7 +2690,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>98</v>
       </c>
@@ -2706,7 +2702,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>99</v>
       </c>
@@ -2718,7 +2714,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>100</v>
       </c>
@@ -2730,7 +2726,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>101</v>
       </c>
@@ -2742,7 +2738,7 @@
         <v>11001</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>102</v>
       </c>
@@ -2754,7 +2750,7 @@
         <v>D54</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>103</v>
       </c>
@@ -2766,7 +2762,7 @@
         <v>6524</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>104</v>
       </c>
@@ -2778,7 +2774,7 @@
         <v>100101</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>105</v>
       </c>
@@ -2790,7 +2786,7 @@
         <v>13330</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>106</v>
       </c>
@@ -2802,7 +2798,7 @@
         <v>32022</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>107</v>
       </c>
@@ -2814,7 +2810,7 @@
         <v>10101</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>108</v>
       </c>
@@ -2826,7 +2822,7 @@
         <v>1802</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>109</v>
       </c>
@@ -2852,9 +2848,9 @@
       <selection activeCell="C3" sqref="A1:G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2865,7 +2861,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>27</v>
       </c>
@@ -2890,7 +2886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>28</v>
       </c>
@@ -2915,7 +2911,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>29</v>
       </c>
@@ -2940,7 +2936,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>30</v>
       </c>
@@ -2952,7 +2948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -2970,9 +2966,9 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2983,7 +2979,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>64</v>
       </c>
@@ -2995,7 +2991,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>65</v>
       </c>
@@ -3007,7 +3003,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>66</v>
       </c>
@@ -3032,9 +3028,9 @@
       <selection activeCell="C2" sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3045,7 +3041,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>25</v>
       </c>
@@ -3057,7 +3053,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>26</v>
       </c>
@@ -3082,9 +3078,9 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3095,7 +3091,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>110</v>
       </c>
@@ -3122,7 +3118,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>111</v>
       </c>
@@ -3149,102 +3145,102 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>131</v>
       </c>
@@ -3262,13 +3258,13 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="11.3984375" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3279,7 +3275,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>88</v>
       </c>
@@ -3291,7 +3287,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>89</v>
       </c>
@@ -3303,7 +3299,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>90</v>
       </c>
@@ -3315,7 +3311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>91</v>
       </c>
@@ -3327,7 +3323,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>92</v>
       </c>
@@ -3336,7 +3332,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>189</v>
       </c>
@@ -3348,7 +3344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>93</v>
       </c>
@@ -3360,7 +3356,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>94</v>
       </c>
@@ -3372,7 +3368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>95</v>
       </c>
@@ -3384,7 +3380,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>188</v>
       </c>
@@ -3396,7 +3392,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>96</v>
       </c>
@@ -3415,13 +3411,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E7F2DB5-7F95-4183-A66F-05B0D65B8106}">
   <dimension ref="A1:O18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="V36" sqref="V36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3453,7 +3449,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>132</v>
       </c>
@@ -3486,7 +3482,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>133</v>
       </c>
@@ -3504,7 +3500,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>134</v>
       </c>
@@ -3522,7 +3518,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>135</v>
       </c>
@@ -3533,7 +3529,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>136</v>
       </c>
@@ -3545,12 +3541,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>138</v>
       </c>
@@ -3562,7 +3558,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>139</v>
       </c>
@@ -3574,37 +3570,37 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>146</v>
       </c>
@@ -3622,9 +3618,9 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3635,7 +3631,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>31</v>
       </c>
@@ -3681,7 +3677,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>32</v>
       </c>
@@ -3727,7 +3723,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -3772,7 +3768,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>34</v>
       </c>

</xml_diff>